<commit_message>
ReBuild Doors and Corners 업데이트
</commit_message>
<xml_diff>
--- a/Data/ReBuild Doors and Corners - 3262718980/3262718980.xlsx
+++ b/Data/ReBuild Doors and Corners - 3262718980/3262718980.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Data\ReBuild Doors and Corners - 3262718980\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\OneDrive\바탕 화면\림월드 번역\ReBuild Doors and Corners - 3262718980\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B1A3110-5384-4036-A3E3-96005782B77F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DAEB7EA-EFE6-47BB-991D-07B85BF82628}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240609" sheetId="1" r:id="rId1"/>
@@ -35,27 +35,60 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>RimWorldKorea</author>
+    <author>bjmi0</author>
   </authors>
   <commentList>
-    <comment ref="F72" authorId="0" shapeId="0" xr:uid="{F2B5F06E-B0F6-4E2E-8B5E-CBA99566E640}">
+    <comment ref="E44" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-07-14 이전의 원문: 'Divides rooms. Powered operation allows people to move through the door without slowing down. Does not block light.'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E72" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-07-14에 삭제됨. 삭제 이전 번역문: '고철 덩어리나 금속이 혼합된 물품에서 금속을 추출하거나, 바위 덩어리를 유리로 가공합니다. 전기가 많이 소비됩니다.'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E74" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-07-14</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
             <family val="3"/>
             <charset val="129"/>
           </rPr>
-          <t>바닐라</t>
+          <t>에</t>
         </r>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -63,14 +96,92 @@
         </r>
         <r>
           <rPr>
-            <b/>
             <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="돋움"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
             <family val="3"/>
             <charset val="129"/>
           </rPr>
-          <t>노드</t>
+          <t>새로</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>추가된</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>노드들</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> (16</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="돋움체"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>개</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F74" authorId="0" shapeId="0" xr:uid="{8155089B-1CA2-4E83-B0CD-023910EBFA45}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>2024-07-14에 새로 추가된 노드들 (16개)</t>
         </r>
       </text>
     </comment>
@@ -79,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="354">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -111,6 +222,9 @@
     <t>General</t>
   </si>
   <si>
+    <t>일반</t>
+  </si>
+  <si>
     <t>ModSettingsFramework.ModOptionCategoryDef+RB_Walls.label</t>
   </si>
   <si>
@@ -123,6 +237,18 @@
     <t>ModSettingsFramework.ModOptionCategoryDef+RB_Doors.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>벽</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>RB_Doors.label</t>
   </si>
   <si>
@@ -132,6 +258,18 @@
     <t>RecipeDef+RB_Make_GlassFromChunks.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>문</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>RecipeDef</t>
   </si>
   <si>
@@ -144,12 +282,27 @@
     <t>RecipeDef+RB_Make_GlassFromChunks.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유리 제작</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>RB_Make_GlassFromChunks.description</t>
   </si>
   <si>
     <t>Refine stone chunks into basic glass.</t>
   </si>
   <si>
+    <t>바위 덩어리를 일반적인 유리로 가공합니다.</t>
+  </si>
+  <si>
     <t>RecipeDef+RB_Make_GlassFromChunks.jobString</t>
   </si>
   <si>
@@ -162,6 +315,18 @@
     <t>RecipeDef+RB_Make_BallisticGlassFromChunks.label</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>유리 제작 중</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>RB_Make_BallisticGlassFromChunks.label</t>
   </si>
   <si>
@@ -171,12 +336,27 @@
     <t>RecipeDef+RB_Make_BallisticGlassFromChunks.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>방탄 유리 제작</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>RB_Make_BallisticGlassFromChunks.description</t>
   </si>
   <si>
     <t>Refine stone chunks and plasteel into ballistic glass.</t>
   </si>
   <si>
+    <t>바위 덩어리와 플라스틸을 섞어 방탄 유리로 가공합니다.</t>
+  </si>
+  <si>
     <t>RecipeDef+RB_Make_BallisticGlassFromChunks.jobString</t>
   </si>
   <si>
@@ -189,6 +369,18 @@
     <t>TerrainDef+RB_FinePlankWood.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>방탄 유리 제작 중</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>TerrainDef</t>
   </si>
   <si>
@@ -198,6 +390,9 @@
     <t>Exquisite wooden tiles, made with no compromises, for expressing economic status. Slow to construct.</t>
   </si>
   <si>
+    <t>원칙을 굽히지 않고 만든 정교한 나무 바닥으로, 경제적인 지위를 나타냅니다. 건설 속도가 느립니다.</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_FinePlankWood.label</t>
   </si>
   <si>
@@ -207,6 +402,9 @@
     <t>fine wood floor</t>
   </si>
   <si>
+    <t>멋진 나무 바닥</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_BurnedFineWoodPlankFloor.label</t>
   </si>
   <si>
@@ -216,6 +414,9 @@
     <t>burned wood floor</t>
   </si>
   <si>
+    <t>불탄 멋진 나무 바닥</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_BurnedFineWoodPlankFloor.description</t>
   </si>
   <si>
@@ -225,6 +426,9 @@
     <t>Burned-out fine wood plank flooring.</t>
   </si>
   <si>
+    <t>불에 탄 멋진 나무 판자 바닥입니다.</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_MetalGrateTile.label</t>
   </si>
   <si>
@@ -234,6 +438,9 @@
     <t>steel grate tile</t>
   </si>
   <si>
+    <t>철제 격자 바닥</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_MetalGrateTile.description</t>
   </si>
   <si>
@@ -243,6 +450,9 @@
     <t>Steel grate tiles, for that spaceship workshop look. They are very quick to clean and get a bonus to cleanliness for use in medical settings.</t>
   </si>
   <si>
+    <t>우주선 느낌의 금속 바닥입니다. 청소하기 쉬운데다 청결도가 추가됩니다.</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_SilverGrateTile.label</t>
   </si>
   <si>
@@ -252,6 +462,9 @@
     <t>silver grate tile</t>
   </si>
   <si>
+    <t>은제 격자 바닥</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_SilverGrateTile.description</t>
   </si>
   <si>
@@ -261,6 +474,9 @@
     <t>For a futuristic but royal look, silver grate tiles fit perfectly into luxurious workshops or armories. They are very quick to clean and get a bonus to cleanliness.</t>
   </si>
   <si>
+    <t>미래지향적이면서 귀족다운 은제 바닥으로 사치스러운 방에도 잘 어울립니다. 청소하기 쉽고 청결도가 추가됩니다.</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_GoldGrateTile.label</t>
   </si>
   <si>
@@ -270,6 +486,9 @@
     <t>gold grate tile</t>
   </si>
   <si>
+    <t>금제 격자 바닥</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_GoldGrateTile.description</t>
   </si>
   <si>
@@ -279,6 +498,9 @@
     <t>For idiotic and overbearing extravagance, nothing beats gold grate tiles. They are exceptionally expensive, and exceptionally beautiful, and people will think you're exceptionally snobbish if you actually live on them. They are very quick to clean and get a bonus to cleanliness.</t>
   </si>
   <si>
+    <t>거만한 사치를 위해서는 금제 바닥만 한 게 없습니다. 인상적일 정도로 비싸지만, 인상적으로 아름다우며 이런 곳에 산다면 사람들이 속물로 생각할 것입니다. 청소하기 쉽고 청결도가 추가됩니다.</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_MetalStuddedTile.label</t>
   </si>
   <si>
@@ -288,6 +510,9 @@
     <t>steel studded tile</t>
   </si>
   <si>
+    <t>철제 단추 바닥</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_MetalStuddedTile.description</t>
   </si>
   <si>
@@ -306,6 +531,9 @@
     <t>silver studded tile</t>
   </si>
   <si>
+    <t>은제 단추 바닥</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_SilverStuddedTile.description</t>
   </si>
   <si>
@@ -324,6 +552,9 @@
     <t>gold studded tile</t>
   </si>
   <si>
+    <t>금제 단추 바닥</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_GoldStuddedTile.description</t>
   </si>
   <si>
@@ -333,6 +564,9 @@
     <t>For overbearing extravagance, few things beat studded gold tiles. They are exceptionally expensive, and exceptionally beautiful, and people will think you're exceptionally snobbish if you actually live on them.</t>
   </si>
   <si>
+    <t>거만한 사치를 위해서는 금제 바닥만 한 게 없습니다. 인상적일 정도로 비싸지만, 인상적으로 아름다우며 이런 곳에 산다면 사람들이 속물로 생각할 것입니다.</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_SterileGrateTile.label</t>
   </si>
   <si>
@@ -342,6 +576,9 @@
     <t>sterile grate tile</t>
   </si>
   <si>
+    <t>향균 격자 바닥</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_SterileGrateTile.description</t>
   </si>
   <si>
@@ -351,6 +588,9 @@
     <t>Sterile grate tiles with special cleanliness-enhancing properties. Extra-clean rooms improve outcomes in hospitals and research labs. This tile is very slow to build, but very quick to clean.</t>
   </si>
   <si>
+    <t>방을 청결하게 유지해야 할 때 도움이 됩니다. 매우 청결한 방에서는 의료 작업과 연구의 결과가 향상됩니다. 건설이 매우 느리지만 청소는 쉽습니다.</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_SterileStuddedTile.label</t>
   </si>
   <si>
@@ -360,6 +600,9 @@
     <t>sterile studded tile</t>
   </si>
   <si>
+    <t>향균 단추 바닥</t>
+  </si>
+  <si>
     <t>TerrainDef+RB_SterileStuddedTile.description</t>
   </si>
   <si>
@@ -381,6 +624,9 @@
     <t>rustic wall</t>
   </si>
   <si>
+    <t>소박한 벽</t>
+  </si>
+  <si>
     <t>ThingDef+RB_RusticWall.description</t>
   </si>
   <si>
@@ -390,6 +636,9 @@
     <t>A simplistic, weak and impassable wall. Capable of holding up a roof.</t>
   </si>
   <si>
+    <t>지나갈 수 없는 벽입니다. 단순하고 약해 보입니다. 지붕을 지지할 수 있습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+RB_OrnateWall.label</t>
   </si>
   <si>
@@ -399,6 +648,9 @@
     <t>ornate wall</t>
   </si>
   <si>
+    <t>화려한 벽</t>
+  </si>
+  <si>
     <t>ThingDef+RB_OrnateWall.description</t>
   </si>
   <si>
@@ -408,6 +660,9 @@
     <t>An intricate and impassable wall, decorated with gold. Capable of holding up a roof, but more fragile than a normal wall. Dignity-focused psycaster will receive a meditation bonus when meditating near them.</t>
   </si>
   <si>
+    <t>지나갈 수 없는 벽입니다. 복잡한 문양과 금으로 장식되어있습니다. 지붕을 지지할 수 있지만 튼튼하진 못합니다. 권위 유형의 초능력자는 근처에서 집중 명상을 할 때 명상 보너스를 얻습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+RB_ClerestoryWall.label</t>
   </si>
   <si>
@@ -417,6 +672,9 @@
     <t>clerestory wall</t>
   </si>
   <si>
+    <t>유리창 벽</t>
+  </si>
+  <si>
     <t>ThingDef+RB_ClerestoryWall.description</t>
   </si>
   <si>
@@ -426,6 +684,9 @@
     <t>An impassable half-glass wall. Capable of holding up a roof, but more fragile than a normal wall. Does not block light, providing a growing bonus to plants near them. Slowly refills peoples outdoor need.</t>
   </si>
   <si>
+    <t>지나갈 수 없는 유리창 벽입니다. 지붕을 지지할 수 있지만 튼튼하진 못합니다. 빛을 차단하지 않아 실내에서도 식물을 키울 수 있습니다. 정착민의 외출 욕구를 천천히 채워줍니다.</t>
+  </si>
+  <si>
     <t>ThingDef+RB_ReinforcedClerestoryWall.label</t>
   </si>
   <si>
@@ -435,6 +696,9 @@
     <t>reinforced clerestory wall</t>
   </si>
   <si>
+    <t>강화 유리창 벽</t>
+  </si>
+  <si>
     <t>ThingDef+RB_ReinforcedClerestoryWall.description</t>
   </si>
   <si>
@@ -444,6 +708,9 @@
     <t>An impassable half-glass wall. Capable of holding up a roof. Does not block light, providing a growing bonus to plants near them. Slowly refills peoples outdoor need.</t>
   </si>
   <si>
+    <t>지나갈 수 없는 강화 유리창 벽입니다. 지붕을 지지할 수 있습니다. 빛을 차단하지 않아 실내에서도 식물을 키울 수 있습니다. 정착민의 외출 욕구를 천천히 채워줍니다.</t>
+  </si>
+  <si>
     <t>ThingDef+RB_GlassWall.label</t>
   </si>
   <si>
@@ -453,6 +720,9 @@
     <t>glass wall</t>
   </si>
   <si>
+    <t>유리벽</t>
+  </si>
+  <si>
     <t>ThingDef+RB_GlassWall.description</t>
   </si>
   <si>
@@ -462,6 +732,9 @@
     <t>An impassable glass wall. Capable of holding up a roof, but far more fragile than a normal wall. Does not block light, providing a growing bonus to plants near them. Slowly refills peoples outdoor need.</t>
   </si>
   <si>
+    <t>지나갈 수 없는 유리벽입니다. 지붕을 지지할 수 있지만 튼튼하진 못합니다. 빛을 차단하지 않아 실내에서도 식물을 키울 수 있습니다. 정착민의 외출 욕구를 천천히 채워줍니다.</t>
+  </si>
+  <si>
     <t>ThingDef+RB_ReinforcedGlassWall.label</t>
   </si>
   <si>
@@ -471,6 +744,9 @@
     <t>reinforced glass wall</t>
   </si>
   <si>
+    <t>강화 유리벽</t>
+  </si>
+  <si>
     <t>ThingDef+RB_ReinforcedGlassWall.description</t>
   </si>
   <si>
@@ -480,6 +756,9 @@
     <t>An impassable reinforced glass wall. Capable of holding up a roof. Does not block light, providing a growing bonus to plants near them. Slowly refills peoples outdoor need.</t>
   </si>
   <si>
+    <t>지나갈 수 없는 강화 유리벽입니다. 지붕을 지지할 수 있습니다. 빛을 차단하지 않아 실내에서도 식물을 키울 수 있습니다. 정착민의 외출 욕구를 천천히 채워줍니다.</t>
+  </si>
+  <si>
     <t>ThingDef+RB_GlassAutodoor.label</t>
   </si>
   <si>
@@ -489,13 +768,16 @@
     <t>glass autodoor</t>
   </si>
   <si>
+    <t>유리 자동문</t>
+  </si>
+  <si>
     <t>ThingDef+RB_GlassAutodoor.description</t>
   </si>
   <si>
     <t>RB_GlassAutodoor.description</t>
   </si>
   <si>
-    <t>Divides rooms. Powered operation allows people to move through the door without slowing down. Does not block light.</t>
+    <t>ModSettingsFramework.ModOptionCategoryDef+RB_Floors.label</t>
   </si>
   <si>
     <t>ThingDef+RB_LargeOrnateDoor.label</t>
@@ -507,6 +789,9 @@
     <t>large ornate door</t>
   </si>
   <si>
+    <t>대형 화려한 문</t>
+  </si>
+  <si>
     <t>ThingDef+RB_LargeOrnateDoor.description</t>
   </si>
   <si>
@@ -516,6 +801,9 @@
     <t>Divides rooms. An intricately-carved door, decorated with gold. This large, heavy door requires adjacent walls to function.</t>
   </si>
   <si>
+    <t>방을 나눕니다. 복잡한 문양과 금으로 장식되어있습니다. 이 거대하고 무거운 문은 이를 지지해주는 벽이 있어야 제대로 사용할 수 있습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+RB_OverwallFireplace.label</t>
   </si>
   <si>
@@ -525,6 +813,9 @@
     <t>wall-mounted fireplace</t>
   </si>
   <si>
+    <t>벽걸이 벽난로</t>
+  </si>
+  <si>
     <t>ThingDef+RB_OverwallFireplace.description</t>
   </si>
   <si>
@@ -534,6 +825,9 @@
     <t>A stone fireplace build into an existing wall. As with all heat sources, it must be placed indoors so it has a closed space to heat. Refuelable with wood.</t>
   </si>
   <si>
+    <t>벽걸이형 석재 벽난로입니다. 다른 열원들과 마찬가지로 방을 덥히기 위해선 밀폐된 공간에 배치되어야 합니다. 나무를 채워넣을 수 있습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+RB_Fireplace.label</t>
   </si>
   <si>
@@ -543,6 +837,9 @@
     <t>fireplace</t>
   </si>
   <si>
+    <t>벽난로</t>
+  </si>
+  <si>
     <t>ThingDef+RB_Fireplace.description</t>
   </si>
   <si>
@@ -552,6 +849,9 @@
     <t>A stone fireplace. As with all heat sources, it must be placed indoors so it has a closed space to heat. Refuelable with wood.</t>
   </si>
   <si>
+    <t>석재 벽난로입니다. 다른 열원들과 마찬가지로 방을 덥히기 위해선 밀폐된 공간에 배치되어야 합니다. 나무를 채워넣을 수 있습니다.</t>
+  </si>
+  <si>
     <t>ThingDef+RB_OverwallArmor.label</t>
   </si>
   <si>
@@ -561,6 +861,9 @@
     <t>wall armor</t>
   </si>
   <si>
+    <t>벽 보호구</t>
+  </si>
+  <si>
     <t>ThingDef+RB_OverwallArmor.description</t>
   </si>
   <si>
@@ -570,6 +873,9 @@
     <t>A durable, reinforced armor that seamlessly integrates with existing walls. Provides enhanced protection against external threats while maintaining structural integrity. It will protect the wall under it from damage until destroyed. Must be constructed on an existing wall.</t>
   </si>
   <si>
+    <t>벽을 강화하는 보호구입니다. 구조적으로 기존 벽과 완벽하게 통합되며 외부 위협에 대한 보호 기능을 강화합니다. 파괴될 때까지 설치된 벽을 손상으로부터 보호합니다. 벽에 설치해야 합니다.</t>
+  </si>
+  <si>
     <t>ThingDef+RB_Glass.label</t>
   </si>
   <si>
@@ -579,6 +885,9 @@
     <t>glass</t>
   </si>
   <si>
+    <t>유리</t>
+  </si>
+  <si>
     <t>ThingDef+RB_Glass.description</t>
   </si>
   <si>
@@ -588,6 +897,9 @@
     <t>Transparent, brittle sheets of silica-based material, widely utilised for windows and various other applications where clarity and rigidity are essential.</t>
   </si>
   <si>
+    <t>투명하고 부서지기 쉬운 실리카 기반 소재입니다. 창문을 포함해 다양한 분야에 널리 활용됩니다.</t>
+  </si>
+  <si>
     <t>ThingDef+RB_BallisticGlass.label</t>
   </si>
   <si>
@@ -597,6 +909,9 @@
     <t>ballistic glass</t>
   </si>
   <si>
+    <t>방탄 유리</t>
+  </si>
+  <si>
     <t>ThingDef+RB_BallisticGlass.description</t>
   </si>
   <si>
@@ -606,6 +921,9 @@
     <t>Toughened, multi-layered transparent armor capable of withstanding bullets and explosions, crucial for protecting high-value targets and ensuring safety in hostile environments.</t>
   </si>
   <si>
+    <t>총알과 폭발을 견디도록 강화된 압축 유리입니다. 자산 보호와 안전을 위해 사용됩니다.</t>
+  </si>
+  <si>
     <t>ThingDef+RB_Filth_GlassShards.label</t>
   </si>
   <si>
@@ -615,6 +933,9 @@
     <t>glass shards</t>
   </si>
   <si>
+    <t>유리 파편</t>
+  </si>
+  <si>
     <t>ThingDef+RB_Filth_BallisticGlassShards.label</t>
   </si>
   <si>
@@ -633,6 +954,9 @@
     <t>metal grate tile</t>
   </si>
   <si>
+    <t>금속 격자 바닥</t>
+  </si>
+  <si>
     <t>DesignatorDropdownGroupDef+RB_Floor_Tile_StuddedMetal.label</t>
   </si>
   <si>
@@ -642,6 +966,9 @@
     <t>metal studded tile</t>
   </si>
   <si>
+    <t>금속 단추 바닥</t>
+  </si>
+  <si>
     <t>ThingDef+RB_LargeSecurityDoor.label</t>
   </si>
   <si>
@@ -654,6 +981,9 @@
     <t>large security door</t>
   </si>
   <si>
+    <t>대형 보안 문</t>
+  </si>
+  <si>
     <t>ThingDef+RB_LargeSecurityDoor.description</t>
   </si>
   <si>
@@ -663,6 +993,9 @@
     <t>A heavily reinforced door. It is slow to open and requires electricity, but is very strong. It's a good choice if you want to keep something dangerous out - or in. The door requires walls on either side to function.</t>
   </si>
   <si>
+    <t>튼튼하게 강화된 문입니다. 느리게 열리며 전기가 필요하지만, 매우 강합니다. 뭔가 위험한 것의 출입을 통제하고 싶다면 좋은 선택일 것입니다. 문이 기능하려면 양쪽에 벽이 필요합니다.</t>
+  </si>
+  <si>
     <t>Keyed+RE.MustPlaceHeaterWithFreeSpaces</t>
   </si>
   <si>
@@ -675,6 +1008,9 @@
     <t>The hot side of the fireplace must be exposed.</t>
   </si>
   <si>
+    <t>벽난로의 열원이 노출되어야 합니다.</t>
+  </si>
+  <si>
     <t>Keyed+RE.SetTerrainEdgesLabel</t>
   </si>
   <si>
@@ -684,6 +1020,9 @@
     <t>Set terrain edges</t>
   </si>
   <si>
+    <t>지형 모서리 설정</t>
+  </si>
+  <si>
     <t>Keyed+RE.SetTerrainEdgesDesc</t>
   </si>
   <si>
@@ -693,6 +1032,9 @@
     <t>Terrain rendered in this area will have custom edges.</t>
   </si>
   <si>
+    <t>이 영역에 렌더링되는 지형에 모서리 설정을 적용합니다.</t>
+  </si>
+  <si>
     <t>Keyed+RE.ResetTerrainEdgesLabel</t>
   </si>
   <si>
@@ -702,6 +1044,9 @@
     <t>Reset terrain edges</t>
   </si>
   <si>
+    <t>지형 모서리 초기화</t>
+  </si>
+  <si>
     <t>Keyed+RE.ResetTerrainEdgesDesc</t>
   </si>
   <si>
@@ -711,6 +1056,9 @@
     <t>Reset custom terrain edge area.</t>
   </si>
   <si>
+    <t>지형 모서리 설정을 초기화합니다.</t>
+  </si>
+  <si>
     <t>Keyed+RE.TerrainEdgeTypeHard</t>
   </si>
   <si>
@@ -720,6 +1068,9 @@
     <t>Hard</t>
   </si>
   <si>
+    <t>단단하게</t>
+  </si>
+  <si>
     <t>Keyed+RE.TerrainEdgeTypeFade</t>
   </si>
   <si>
@@ -729,6 +1080,9 @@
     <t>Fade</t>
   </si>
   <si>
+    <t>희미하게</t>
+  </si>
+  <si>
     <t>Keyed+RE.TerrainEdgeTypeFadeRough</t>
   </si>
   <si>
@@ -738,6 +1092,9 @@
     <t>Fade (rough)</t>
   </si>
   <si>
+    <t>희미하게 (거침)</t>
+  </si>
+  <si>
     <t>Keyed+RE.WallArmorMustBePlacedOnWall</t>
   </si>
   <si>
@@ -747,226 +1104,248 @@
     <t>Wall armor requires pre-existing wall to be constructed.</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>ThingDef</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>벽 위에 설치해야 합니다.</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>ThingDef+ElectricSmelter.description</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>ElectricSmelter.description</t>
   </si>
   <si>
     <t>Extracts usable metal from slag chunks and other mixed metal items, as well as refines stone chunks into glass. Consumes a lot of power.</t>
   </si>
   <si>
-    <t>희미하게 (거침)</t>
-  </si>
-  <si>
-    <t>희미하게</t>
-  </si>
-  <si>
-    <t>단단하게</t>
-  </si>
-  <si>
-    <t>지형 모서리 설정을 초기화합니다.</t>
-  </si>
-  <si>
-    <t>지형 모서리 초기화</t>
-  </si>
-  <si>
-    <t>이 영역에 렌더링되는 지형에 모서리 설정을 적용합니다.</t>
-  </si>
-  <si>
-    <t>지형 모서리 설정</t>
-  </si>
-  <si>
-    <t>벽난로의 열원이 노출되어야 합니다.</t>
-  </si>
-  <si>
-    <t>튼튼하게 강화된 문입니다. 느리게 열리며 전기가 필요하지만, 매우 강합니다. 뭔가 위험한 것의 출입을 통제하고 싶다면 좋은 선택일 것입니다. 문이 기능하려면 양쪽에 벽이 필요합니다.</t>
-  </si>
-  <si>
-    <t>대형 보안 문</t>
-  </si>
-  <si>
-    <t>유리 파편</t>
-  </si>
-  <si>
-    <t>총알과 폭발을 견디도록 강화된 압축 유리입니다. 자산 보호와 안전을 위해 사용됩니다.</t>
-  </si>
-  <si>
-    <t>방탄 유리</t>
-  </si>
-  <si>
-    <t>투명하고 부서지기 쉬운 실리카 기반 소재입니다. 창문을 포함해 다양한 분야에 널리 활용됩니다.</t>
-  </si>
-  <si>
-    <t>유리</t>
-  </si>
-  <si>
-    <t>벽을 강화하는 보호구입니다. 구조적으로 기존 벽과 완벽하게 통합되며 외부 위협에 대한 보호 기능을 강화합니다. 파괴될 때까지 설치된 벽을 손상으로부터 보호합니다. 벽에 설치해야 합니다.</t>
-  </si>
-  <si>
-    <t>벽 보호구</t>
-  </si>
-  <si>
-    <t>석재 벽난로입니다. 다른 열원들과 마찬가지로 방을 덥히기 위해선 밀폐된 공간에 배치되어야 합니다. 나무를 채워넣을 수 있습니다.</t>
-  </si>
-  <si>
-    <t>벽난로</t>
-  </si>
-  <si>
-    <t>벽걸이형 석재 벽난로입니다. 다른 열원들과 마찬가지로 방을 덥히기 위해선 밀폐된 공간에 배치되어야 합니다. 나무를 채워넣을 수 있습니다.</t>
-  </si>
-  <si>
-    <t>벽걸이 벽난로</t>
-  </si>
-  <si>
-    <t>방을 나눕니다. 복잡한 문양과 금으로 장식되어있습니다. 이 거대하고 무거운 문은 이를 지지해주는 벽이 있어야 제대로 사용할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>대형 화려한 문</t>
+    <t>RB_Floors.label</t>
+  </si>
+  <si>
+    <t>Divides rooms. Powered operation allows people to move through the door without slowing down.</t>
+  </si>
+  <si>
+    <t>Floors</t>
+  </si>
+  <si>
+    <t>ModSettingsFramework.ModOptionCategoryDef+RB_Integrations.label</t>
+  </si>
+  <si>
+    <t>RB_Integrations.label</t>
+  </si>
+  <si>
+    <t>Mod Integrations</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_FloorLamp.label</t>
+  </si>
+  <si>
+    <t>RB_FloorLamp.label</t>
+  </si>
+  <si>
+    <t>floor lamp</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_FloorLamp.description</t>
+  </si>
+  <si>
+    <t>RB_FloorLamp.description</t>
+  </si>
+  <si>
+    <t>A floor-mounted lamp that lights an area using electricity. It is less powerful than a standing lamp, but can be build on any floor.</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_ReinforcedGlassAutodoor.label</t>
+  </si>
+  <si>
+    <t>RB_ReinforcedGlassAutodoor.label</t>
+  </si>
+  <si>
+    <t>reinforced glass autodoor</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_ReinforcedGlassAutodoor.description</t>
+  </si>
+  <si>
+    <t>RB_ReinforcedGlassAutodoor.description</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_DoubleDoor.label</t>
+  </si>
+  <si>
+    <t>RB_DoubleDoor.label</t>
+  </si>
+  <si>
+    <t>double door</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_DoubleDoor.description</t>
+  </si>
+  <si>
+    <t>RB_DoubleDoor.description</t>
+  </si>
+  <si>
+    <t>Divides rooms. Simple doors must be manually opened, which slows people down. The amount of slowdown depends on what the door is made of.</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_DoubleAutodoor.label</t>
+  </si>
+  <si>
+    <t>RB_DoubleAutodoor.label</t>
+  </si>
+  <si>
+    <t>double autodoor</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_DoubleAutodoor.description</t>
+  </si>
+  <si>
+    <t>RB_DoubleAutodoor.description</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_ACUnitFloor.label</t>
+  </si>
+  <si>
+    <t>RB_ACUnitFloor.label</t>
+  </si>
+  <si>
+    <t>Vanilla Temperature Expanded</t>
+  </si>
+  <si>
+    <t>floor AC unit</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_ACUnitFloor.description</t>
+  </si>
+  <si>
+    <t>RB_ACUnitFloor.description</t>
+  </si>
+  <si>
+    <t>An air-conditioning machine that fits into a floor tile. Emits either cool or warm air in the same direction, depending on the current temperature of the room. Unless unlinked from the network settings, it will aim to achieve the temperature specified in the AC control unit. Needs to be connected to the AC control unit via air ducts.</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_Ship_Beam_Glass.label</t>
+  </si>
+  <si>
+    <t>RB_Ship_Beam_Glass.label</t>
+  </si>
+  <si>
+    <t>Save Our Ship 2</t>
+  </si>
+  <si>
+    <t>ship hull (glass)</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_Ship_Beam_Glass.description</t>
+  </si>
+  <si>
+    <t>RB_Ship_Beam_Glass.description</t>
+  </si>
+  <si>
+    <t>The outer structural elements of a ship's hull. Does not include conduits for power or coolant.</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_Ship_Beam_Viewport.label</t>
+  </si>
+  <si>
+    <t>RB_Ship_Beam_Viewport.label</t>
+  </si>
+  <si>
+    <t>ship hull (viewport)</t>
+  </si>
+  <si>
+    <t>ThingDef+RB_Ship_Beam_Viewport.description</t>
+  </si>
+  <si>
+    <t>RB_Ship_Beam_Viewport.description</t>
+  </si>
+  <si>
+    <t>바닥</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>모드 통합</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>바닥등</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>전기를 사용하여 공간을 밝히는 바닥 설치형 전등입니다. 일반 전등보다 덜 강력하지만 어떤 바닥에도 설치할 수 있습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>강화 유리 자동문</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>방을 나눕니다. 전기로 작동하며 문 통과시 이동속도 감소가 적거나 없습니다.</t>
+  </si>
+  <si>
+    <t>방을 나눕니다. 전기로 작동하며 문 통과시 이동속도 감소가 적거나 없습니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이중문</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이중 자동문</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>방을 나눕니다. 수동으로 열고 닫으며 문 통과시 이동속도가 느려집니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>방을 나눕니다. 전기로 작동하며 문 통과시 이동속도 감소가 적거나 없습니다. 빛을 차단하지 않습니다.</t>
-  </si>
-  <si>
-    <t>유리 자동문</t>
-  </si>
-  <si>
-    <t>지나갈 수 없는 강화 유리벽입니다. 지붕을 지지할 수 있습니다. 빛을 차단하지 않아 실내에서도 식물을 키울 수 있습니다. 정착민의 외출 욕구를 천천히 채워줍니다.</t>
-  </si>
-  <si>
-    <t>강화 유리벽</t>
-  </si>
-  <si>
-    <t>지나갈 수 없는 유리벽입니다. 지붕을 지지할 수 있지만 튼튼하진 못합니다. 빛을 차단하지 않아 실내에서도 식물을 키울 수 있습니다. 정착민의 외출 욕구를 천천히 채워줍니다.</t>
-  </si>
-  <si>
-    <t>유리벽</t>
-  </si>
-  <si>
-    <t>지나갈 수 없는 강화 유리창 벽입니다. 지붕을 지지할 수 있습니다. 빛을 차단하지 않아 실내에서도 식물을 키울 수 있습니다. 정착민의 외출 욕구를 천천히 채워줍니다.</t>
-  </si>
-  <si>
-    <t>강화 유리창 벽</t>
-  </si>
-  <si>
-    <t>지나갈 수 없는 유리창 벽입니다. 지붕을 지지할 수 있지만 튼튼하진 못합니다. 빛을 차단하지 않아 실내에서도 식물을 키울 수 있습니다. 정착민의 외출 욕구를 천천히 채워줍니다.</t>
-  </si>
-  <si>
-    <t>유리창 벽</t>
-  </si>
-  <si>
-    <t>지나갈 수 없는 벽입니다. 복잡한 문양과 금으로 장식되어있습니다. 지붕을 지지할 수 있지만 튼튼하진 못합니다. 권위 유형의 초능력자는 근처에서 집중 명상을 할 때 명상 보너스를 얻습니다.</t>
-  </si>
-  <si>
-    <t>화려한 벽</t>
-  </si>
-  <si>
-    <t>지나갈 수 없는 벽입니다. 단순하고 약해 보입니다. 지붕을 지지할 수 있습니다.</t>
-  </si>
-  <si>
-    <t>소박한 벽</t>
-  </si>
-  <si>
-    <t>방을 청결하게 유지해야 할 때 도움이 됩니다. 매우 청결한 방에서는 의료 작업과 연구의 결과가 향상됩니다. 건설이 매우 느리지만 청소는 쉽습니다.</t>
-  </si>
-  <si>
-    <t>향균 단추 바닥</t>
-  </si>
-  <si>
-    <t>향균 격자 바닥</t>
-  </si>
-  <si>
-    <t>거만한 사치를 위해서는 금제 바닥만 한 게 없습니다. 인상적일 정도로 비싸지만, 인상적으로 아름다우며 이런 곳에 산다면 사람들이 속물로 생각할 것입니다.</t>
-  </si>
-  <si>
-    <t>금제 단추 바닥</t>
-  </si>
-  <si>
-    <t>미래지향적이면서 귀족다운 은제 바닥으로 사치스러운 방에도 잘 어울립니다. 청소하기 쉽고 청결도가 추가됩니다.</t>
-  </si>
-  <si>
-    <t>은제 단추 바닥</t>
-  </si>
-  <si>
-    <t>우주선 느낌의 금속 바닥입니다. 청소하기 쉬운데다 청결도가 추가됩니다.</t>
-  </si>
-  <si>
-    <t>철제 단추 바닥</t>
-  </si>
-  <si>
-    <t>거만한 사치를 위해서는 금제 바닥만 한 게 없습니다. 인상적일 정도로 비싸지만, 인상적으로 아름다우며 이런 곳에 산다면 사람들이 속물로 생각할 것입니다. 청소하기 쉽고 청결도가 추가됩니다.</t>
-  </si>
-  <si>
-    <t>금제 격자 바닥</t>
-  </si>
-  <si>
-    <t>은제 격자 바닥</t>
-  </si>
-  <si>
-    <t>철제 격자 바닥</t>
-  </si>
-  <si>
-    <t>불에 탄 멋진 나무 판자 바닥입니다.</t>
-  </si>
-  <si>
-    <t>불탄 멋진 나무 바닥</t>
-  </si>
-  <si>
-    <t>멋진 나무 바닥</t>
-  </si>
-  <si>
-    <t>원칙을 굽히지 않고 만든 정교한 나무 바닥으로, 경제적인 지위를 나타냅니다. 건설 속도가 느립니다.</t>
-  </si>
-  <si>
-    <t>바위 덩어리와 플라스틸을 섞어 방탄 유리로 가공합니다.</t>
-  </si>
-  <si>
-    <t>바위 덩어리를 일반적인 유리로 가공합니다.</t>
-  </si>
-  <si>
-    <t>일반</t>
-  </si>
-  <si>
-    <t>금속 단추 바닥</t>
-  </si>
-  <si>
-    <t>금속 격자 바닥</t>
-  </si>
-  <si>
-    <t>벽</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>문</t>
+    <t>바닥 냉방기</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>유리 제작</t>
+    <t>바닥에 설치할 수 있는 냉방기입니다. 방의 현재 온도에 따라서 뜨겁거나 찬 공기를 같은 방향으로 내보낼 수 있습니다.\n\n독립 제어 모드로 설정하지 않으면 방의 온도를 중앙 제어기에서 지정한 온도에 맞추려고 할 것입니다. 공조 파이프를 통해 공조 제어기와 연결되어야 합니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>유리 제작 중</t>
+    <t>함선의 외부 골조입니다. 전선 및 냉각 배관이 포함되지 않았습니다.</t>
+  </si>
+  <si>
+    <t>선체 (유리)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>방탄 유리 제작</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>방탄 유리 제작 중</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>벽 위에 설치해야 합니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>고철 덩어리나 금속이 혼합된 물품에서 금속을 추출하거나, 바위 덩어리를 유리로 가공합니다. 전기가 많이 소비됩니다.</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ThingDef+ElectricSmelter.description</t>
+    <t>선체 (전망창)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -994,27 +1373,40 @@
       <charset val="129"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
+      <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
-      <color indexed="81"/>
-      <name val="돋움"/>
+      <color rgb="FF000000"/>
+      <name val="돋움체"/>
       <family val="3"/>
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA500"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF87CEEB"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1029,9 +1421,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1334,10 +1729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F72"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K65" sqref="K65"/>
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -1348,7 +1743,8 @@
     <col min="4" max="4" width="29.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="48.6328125" style="1" customWidth="1"/>
     <col min="6" max="6" width="36.453125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -1385,1203 +1781,1490 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>280</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>283</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>284</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A5" s="1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>285</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>279</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>286</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>287</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A9" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>278</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>288</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>277</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>276</v>
+        <v>52</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>275</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A14" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="C14" s="1" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>274</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>273</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>52</v>
+        <v>66</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>67</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>268</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="1" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>272</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A18" s="1" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>266</v>
+        <v>76</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>271</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A20" s="1" t="s">
-        <v>63</v>
+        <v>81</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>270</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A21" s="1" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>269</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A22" s="1" t="s">
-        <v>69</v>
+        <v>89</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>70</v>
+        <v>90</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>268</v>
+        <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A23" s="1" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>73</v>
+        <v>93</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>74</v>
+        <v>94</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>267</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A24" s="1" t="s">
-        <v>75</v>
+        <v>96</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A25" s="1" t="s">
-        <v>78</v>
+        <v>99</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>80</v>
+        <v>101</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>265</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A26" s="1" t="s">
-        <v>81</v>
+        <v>103</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>83</v>
+        <v>105</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>264</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A27" s="1" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>85</v>
+        <v>108</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>86</v>
+        <v>109</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>263</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A28" s="1" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>88</v>
+        <v>112</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>89</v>
+        <v>113</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>261</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
-        <v>90</v>
+        <v>115</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>91</v>
+        <v>116</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>92</v>
+        <v>117</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>262</v>
+        <v>118</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A30" s="1" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>94</v>
+        <v>120</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>95</v>
+        <v>121</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>261</v>
+        <v>114</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A31" s="1" t="s">
-        <v>96</v>
+        <v>122</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>98</v>
+        <v>124</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>260</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A32" s="1" t="s">
-        <v>100</v>
+        <v>127</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>101</v>
+        <v>128</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>102</v>
+        <v>129</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>259</v>
+        <v>130</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A33" s="1" t="s">
-        <v>103</v>
+        <v>131</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>104</v>
+        <v>132</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>258</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A34" s="1" t="s">
-        <v>106</v>
+        <v>135</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>107</v>
+        <v>136</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>108</v>
+        <v>137</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>257</v>
+        <v>138</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="1" t="s">
-        <v>109</v>
+        <v>139</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>110</v>
+        <v>140</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>111</v>
+        <v>141</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>256</v>
+        <v>142</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="1" t="s">
-        <v>112</v>
+        <v>143</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>113</v>
+        <v>144</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>114</v>
+        <v>145</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>255</v>
+        <v>146</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A37" s="1" t="s">
-        <v>115</v>
+        <v>147</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>116</v>
+        <v>148</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>117</v>
+        <v>149</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>254</v>
+        <v>150</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
-        <v>118</v>
+        <v>151</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>119</v>
+        <v>152</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>120</v>
+        <v>153</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>253</v>
+        <v>154</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="1" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>122</v>
+        <v>156</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>123</v>
+        <v>157</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>252</v>
+        <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A40" s="1" t="s">
-        <v>124</v>
+        <v>159</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>125</v>
+        <v>160</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>126</v>
+        <v>161</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>251</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>127</v>
+        <v>163</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>128</v>
+        <v>164</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>129</v>
+        <v>165</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>250</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A42" s="1" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>131</v>
+        <v>168</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>132</v>
+        <v>169</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>249</v>
+        <v>170</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A43" s="1" t="s">
-        <v>133</v>
+        <v>171</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>134</v>
+        <v>172</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>135</v>
+        <v>173</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>248</v>
+        <v>174</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A44" s="1" t="s">
-        <v>136</v>
+        <v>175</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>138</v>
+        <v>176</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>292</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>247</v>
+        <v>348</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="1" t="s">
-        <v>139</v>
+        <v>178</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>140</v>
+        <v>179</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>141</v>
+        <v>180</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>246</v>
+        <v>181</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
-        <v>142</v>
+        <v>182</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>144</v>
+        <v>184</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>245</v>
+        <v>185</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A47" s="1" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>146</v>
+        <v>187</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>147</v>
+        <v>188</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>244</v>
+        <v>189</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A48" s="1" t="s">
-        <v>148</v>
+        <v>190</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>149</v>
+        <v>191</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>150</v>
+        <v>192</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>243</v>
+        <v>193</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A49" s="1" t="s">
-        <v>151</v>
+        <v>194</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>152</v>
+        <v>195</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>153</v>
+        <v>196</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>242</v>
+        <v>197</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A50" s="1" t="s">
-        <v>154</v>
+        <v>198</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>155</v>
+        <v>199</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>156</v>
+        <v>200</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>241</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A51" s="1" t="s">
-        <v>157</v>
+        <v>202</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>158</v>
+        <v>203</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>240</v>
+        <v>205</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A52" s="1" t="s">
-        <v>160</v>
+        <v>206</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>161</v>
+        <v>207</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>162</v>
+        <v>208</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>239</v>
+        <v>209</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A53" s="1" t="s">
-        <v>163</v>
+        <v>210</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>164</v>
+        <v>211</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>165</v>
+        <v>212</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>238</v>
+        <v>213</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A54" s="1" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>167</v>
+        <v>215</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>168</v>
+        <v>216</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>237</v>
+        <v>217</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A55" s="1" t="s">
-        <v>169</v>
+        <v>218</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>170</v>
+        <v>219</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>171</v>
+        <v>220</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A56" s="1" t="s">
-        <v>172</v>
+        <v>222</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>173</v>
+        <v>223</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>174</v>
+        <v>224</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A57" s="1" t="s">
-        <v>175</v>
+        <v>226</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>176</v>
+        <v>227</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>177</v>
+        <v>228</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A58" s="1" t="s">
-        <v>178</v>
+        <v>230</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>179</v>
+        <v>231</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>177</v>
+        <v>228</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A59" s="1" t="s">
-        <v>180</v>
+        <v>232</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>181</v>
+        <v>233</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>182</v>
+        <v>234</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>183</v>
+        <v>235</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>282</v>
+        <v>236</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A60" s="1" t="s">
-        <v>184</v>
+        <v>237</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>181</v>
+        <v>233</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>185</v>
+        <v>238</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>186</v>
+        <v>239</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>281</v>
+        <v>240</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A61" s="1" t="s">
-        <v>187</v>
+        <v>241</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>188</v>
+        <v>242</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>189</v>
+        <v>243</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>190</v>
+        <v>244</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A62" s="1" t="s">
-        <v>191</v>
+        <v>246</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>97</v>
+        <v>123</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>192</v>
+        <v>247</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>189</v>
+        <v>243</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>193</v>
+        <v>248</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A63" s="1" t="s">
-        <v>194</v>
+        <v>250</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>196</v>
+        <v>252</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>197</v>
+        <v>253</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>231</v>
+        <v>254</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A64" s="1" t="s">
-        <v>198</v>
+        <v>255</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>199</v>
+        <v>256</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>200</v>
+        <v>257</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>230</v>
+        <v>258</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
-        <v>201</v>
+        <v>259</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>202</v>
+        <v>260</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>203</v>
+        <v>261</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>229</v>
+        <v>262</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A66" s="1" t="s">
-        <v>204</v>
+        <v>263</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>205</v>
+        <v>264</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>206</v>
+        <v>265</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>228</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A67" s="1" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>208</v>
+        <v>268</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>209</v>
+        <v>269</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>227</v>
+        <v>270</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A68" s="1" t="s">
-        <v>210</v>
+        <v>271</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>211</v>
+        <v>272</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>212</v>
+        <v>273</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>226</v>
+        <v>274</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>213</v>
+        <v>275</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>214</v>
+        <v>276</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>215</v>
+        <v>277</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>225</v>
+        <v>278</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>216</v>
+        <v>279</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>217</v>
+        <v>280</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>218</v>
+        <v>281</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>224</v>
+        <v>282</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>219</v>
+        <v>283</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>195</v>
+        <v>251</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>220</v>
+        <v>284</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>221</v>
+        <v>285</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="E72" s="3" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A74" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="F74" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A75" s="1" t="s">
+        <v>294</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>296</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A76" s="1" t="s">
+        <v>297</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>298</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>299</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A77" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>301</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A78" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A79" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="E79" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="B72" s="1" t="s">
-        <v>291</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>290</v>
+      <c r="F79" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A80" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A81" s="1" t="s">
+        <v>311</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>312</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>313</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A82" s="1" t="s">
+        <v>314</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A83" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>318</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A84" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="B84" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>320</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>322</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A85" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>324</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A86" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C86" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A87" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F87" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A88" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C88" s="1" t="s">
+        <v>334</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E88" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A89" s="1" t="s">
+        <v>336</v>
+      </c>
+      <c r="B89" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="E89" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="F89" s="1" t="s">
+        <v>351</v>
       </c>
     </row>
   </sheetData>

</xml_diff>